<commit_message>
Full function names, more mapfile metadata.
</commit_message>
<xml_diff>
--- a/samples/ubiome/ubiome-processed-outputs/json/frat_map_file.xlsx
+++ b/samples/ubiome/ubiome-processed-outputs/json/frat_map_file.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>SSR</t>
   </si>
@@ -20,6 +20,9 @@
     <t>id</t>
   </si>
   <si>
+    <t>Site</t>
+  </si>
+  <si>
     <t>FJ5 - gut</t>
   </si>
   <si>
@@ -48,6 +51,12 @@
   </si>
   <si>
     <t>FJ4 - gut</t>
+  </si>
+  <si>
+    <t>Gut</t>
+  </si>
+  <si>
+    <t>Spare</t>
   </si>
 </sst>
 </file>
@@ -105,13 +114,19 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>300909.0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
@@ -119,7 +134,10 @@
         <v>300921.0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -127,7 +145,10 @@
         <v>300945.0</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -135,7 +156,10 @@
         <v>300948.0</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -143,7 +167,10 @@
         <v>300960.0</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -151,7 +178,10 @@
         <v>300975.0</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -159,7 +189,10 @@
         <v>300987.0</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -167,7 +200,10 @@
         <v>301026.0</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -175,7 +211,10 @@
         <v>301029.0</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -183,7 +222,10 @@
         <v>301032.0</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>